<commit_message>
updated species trait code
</commit_message>
<xml_diff>
--- a/data/butterfly.date.outlier.notes.xlsx
+++ b/data/butterfly.date.outlier.notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhamo\Documents\git\nc-butterfly-phenology\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F858A775-773A-4395-91F1-5925F862D0A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE6BC42-4DA1-4E99-82FD-79A8E17C0581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="417" activeTab="1" xr2:uid="{AFBB4C1E-9820-474D-A61E-6E962BF62D18}"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="19180" windowHeight="10200" tabRatio="417" xr2:uid="{AFBB4C1E-9820-474D-A61E-6E962BF62D18}"/>
   </bookViews>
   <sheets>
     <sheet name="notes by species" sheetId="2" r:id="rId1"/>
@@ -347,9 +347,6 @@
     <t>Thorybes bathyllus</t>
   </si>
   <si>
-    <t>Vanessa atalantis</t>
-  </si>
-  <si>
     <t>Wallengrenia otho</t>
   </si>
   <si>
@@ -543,6 +540,9 @@
   </si>
   <si>
     <t>CL archive starts in 2003 - need to consult HL for earlier years</t>
+  </si>
+  <si>
+    <t>Vanessa atalanta</t>
   </si>
 </sst>
 </file>
@@ -921,11 +921,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F81EFF3C-CDDE-41B0-A824-6179CE9B7230}">
   <dimension ref="A1:X48"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A39" sqref="A39"/>
+      <selection pane="bottomRight" activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -937,7 +937,7 @@
     <col min="5" max="5" width="11.7265625" customWidth="1"/>
     <col min="6" max="6" width="16.90625" customWidth="1"/>
     <col min="7" max="7" width="13" style="3" customWidth="1"/>
-    <col min="8" max="9" width="13" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="21.90625" style="5" customWidth="1"/>
     <col min="11" max="12" width="17.81640625" customWidth="1"/>
     <col min="13" max="13" width="17.36328125" customWidth="1"/>
@@ -974,7 +974,7 @@
         <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>38</v>
@@ -983,7 +983,7 @@
         <v>40</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>27</v>
@@ -1059,7 +1059,7 @@
         <v>42</v>
       </c>
       <c r="K2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L2">
         <v>13</v>
@@ -1238,7 +1238,7 @@
         <v>41</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="V4" t="s">
         <v>41</v>
@@ -1463,7 +1463,7 @@
         <v>41</v>
       </c>
       <c r="W7" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.35">
@@ -1535,7 +1535,7 @@
         <v>41</v>
       </c>
       <c r="W8" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.35">
@@ -1601,7 +1601,7 @@
         <v>41</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="W9" s="5" t="s">
         <v>41</v>
@@ -1716,7 +1716,7 @@
         <v>45</v>
       </c>
       <c r="K11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L11">
         <v>16</v>
@@ -1967,7 +1967,7 @@
         <v>71.36</v>
       </c>
       <c r="S14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U14" s="3" t="s">
         <v>41</v>
@@ -1976,7 +1976,7 @@
         <v>41</v>
       </c>
       <c r="W14" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.35">
@@ -2039,10 +2039,10 @@
         <v>95.45</v>
       </c>
       <c r="S15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="U15" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="W15" s="5" t="s">
         <v>41</v>
@@ -2072,7 +2072,7 @@
         <v>43</v>
       </c>
       <c r="H16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I16">
         <f t="shared" si="1"/>
@@ -2232,10 +2232,10 @@
         <v>204.17</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L18">
         <v>10</v>
@@ -2270,7 +2270,7 @@
         <v>41</v>
       </c>
       <c r="W18" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.35">
@@ -2333,7 +2333,7 @@
         <v>74.41</v>
       </c>
       <c r="S19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U19" s="3" t="s">
         <v>41</v>
@@ -2342,7 +2342,7 @@
         <v>41</v>
       </c>
       <c r="W19" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.35">
@@ -2483,7 +2483,7 @@
         <v>2017</v>
       </c>
       <c r="U21" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="W21" s="5" t="s">
         <v>41</v>
@@ -2783,7 +2783,7 @@
         <v>41</v>
       </c>
       <c r="W25" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.35">
@@ -3002,7 +3002,7 @@
         <v>41</v>
       </c>
       <c r="W28" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.35">
@@ -3587,7 +3587,7 @@
         <v>2020</v>
       </c>
       <c r="U36" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="W36" s="5" t="s">
         <v>41</v>
@@ -3737,7 +3737,7 @@
         <v>41</v>
       </c>
       <c r="W38" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.35">
@@ -3771,10 +3771,10 @@
         <v>121.84</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L39">
         <v>10</v>
@@ -3809,7 +3809,7 @@
         <v>41</v>
       </c>
       <c r="W39" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.35">
@@ -3843,10 +3843,10 @@
         <v>123.73</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L40">
         <v>15</v>
@@ -3872,7 +3872,7 @@
         <v>68.37</v>
       </c>
       <c r="S40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U40" s="3" t="s">
         <v>41</v>
@@ -3881,7 +3881,7 @@
         <v>41</v>
       </c>
       <c r="W40" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.35">
@@ -3918,7 +3918,7 @@
         <v>44</v>
       </c>
       <c r="K41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L41">
         <v>10</v>
@@ -4244,7 +4244,7 @@
         <v>41</v>
       </c>
       <c r="U45" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W45" s="5" t="s">
         <v>41</v>
@@ -4252,7 +4252,7 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>103</v>
+        <v>168</v>
       </c>
       <c r="B46">
         <v>93</v>
@@ -4319,7 +4319,7 @@
         <v>41</v>
       </c>
       <c r="W46" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.35">
@@ -4399,7 +4399,7 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B48">
         <v>127</v>
@@ -4460,7 +4460,7 @@
         <v>2010</v>
       </c>
       <c r="U48" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="W48" s="5" t="s">
         <v>41</v>
@@ -4478,9 +4478,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF978CEF-4D9C-417C-A460-67F4EE090377}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4490,7 +4490,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -4501,13 +4501,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -4515,10 +4515,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1996</v>
+        <v>1993</v>
       </c>
       <c r="C4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -4526,13 +4526,13 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>2005</v>
+        <v>1994</v>
       </c>
       <c r="C5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -4540,16 +4540,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2019</v>
+        <v>1996</v>
       </c>
       <c r="C6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -4557,10 +4557,10 @@
         <v>81</v>
       </c>
       <c r="B7">
-        <v>2017</v>
+        <v>1997</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -4568,13 +4568,13 @@
         <v>82</v>
       </c>
       <c r="B8">
-        <v>2020</v>
+        <v>1997</v>
       </c>
       <c r="C8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -4582,13 +4582,13 @@
         <v>83</v>
       </c>
       <c r="B9">
-        <v>2009</v>
+        <v>2000</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -4596,13 +4596,13 @@
         <v>84</v>
       </c>
       <c r="B10">
-        <v>2006</v>
+        <v>2000</v>
       </c>
       <c r="C10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -4610,13 +4610,13 @@
         <v>85</v>
       </c>
       <c r="B11">
-        <v>2017</v>
+        <v>2000</v>
       </c>
       <c r="C11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -4624,13 +4624,13 @@
         <v>25</v>
       </c>
       <c r="B12">
-        <v>2011</v>
+        <v>2000</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -4638,13 +4638,13 @@
         <v>21</v>
       </c>
       <c r="B13">
-        <v>2019</v>
+        <v>2001</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -4652,13 +4652,13 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <v>2020</v>
+        <v>2005</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -4666,13 +4666,13 @@
         <v>6</v>
       </c>
       <c r="B15">
-        <v>2012</v>
+        <v>2005</v>
       </c>
       <c r="C15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -4683,10 +4683,10 @@
         <v>2005</v>
       </c>
       <c r="C16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -4694,13 +4694,13 @@
         <v>87</v>
       </c>
       <c r="B17">
-        <v>2012</v>
+        <v>2006</v>
       </c>
       <c r="C17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -4708,10 +4708,10 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>1997</v>
+        <v>2007</v>
       </c>
       <c r="C18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -4719,10 +4719,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>2000</v>
+        <v>2007</v>
       </c>
       <c r="C19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -4730,13 +4730,13 @@
         <v>15</v>
       </c>
       <c r="B20">
-        <v>2013</v>
+        <v>2009</v>
       </c>
       <c r="C20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -4744,10 +4744,10 @@
         <v>88</v>
       </c>
       <c r="B21">
-        <v>1997</v>
+        <v>2011</v>
       </c>
       <c r="C21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -4755,10 +4755,10 @@
         <v>88</v>
       </c>
       <c r="B22">
-        <v>2015</v>
+        <v>2011</v>
       </c>
       <c r="C22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -4766,10 +4766,10 @@
         <v>89</v>
       </c>
       <c r="B23">
-        <v>1994</v>
+        <v>2012</v>
       </c>
       <c r="C23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -4777,10 +4777,10 @@
         <v>10</v>
       </c>
       <c r="B24">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="C24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -4788,10 +4788,10 @@
         <v>90</v>
       </c>
       <c r="B25">
-        <v>2007</v>
+        <v>2012</v>
       </c>
       <c r="C25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -4799,13 +4799,13 @@
         <v>3</v>
       </c>
       <c r="B26">
-        <v>2005</v>
+        <v>2012</v>
       </c>
       <c r="C26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -4813,10 +4813,10 @@
         <v>92</v>
       </c>
       <c r="B27">
-        <v>2000</v>
+        <v>2013</v>
       </c>
       <c r="C27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -4824,10 +4824,10 @@
         <v>5</v>
       </c>
       <c r="B28">
-        <v>2000</v>
+        <v>2013</v>
       </c>
       <c r="C28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -4835,10 +4835,10 @@
         <v>94</v>
       </c>
       <c r="B29">
-        <v>2001</v>
+        <v>2014</v>
       </c>
       <c r="C29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -4846,13 +4846,13 @@
         <v>11</v>
       </c>
       <c r="B30">
-        <v>2020</v>
+        <v>2014</v>
       </c>
       <c r="C30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -4860,13 +4860,13 @@
         <v>26</v>
       </c>
       <c r="B31">
-        <v>2007</v>
+        <v>2015</v>
       </c>
       <c r="C31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -4874,10 +4874,10 @@
         <v>7</v>
       </c>
       <c r="B32">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="C32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -4885,13 +4885,13 @@
         <v>22</v>
       </c>
       <c r="B33">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="C33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -4899,16 +4899,16 @@
         <v>96</v>
       </c>
       <c r="B34">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="C34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -4916,13 +4916,13 @@
         <v>9</v>
       </c>
       <c r="B35">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -4930,13 +4930,13 @@
         <v>97</v>
       </c>
       <c r="B36">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C36" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -4944,10 +4944,10 @@
         <v>98</v>
       </c>
       <c r="B37">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="C37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -4955,10 +4955,10 @@
         <v>98</v>
       </c>
       <c r="B38">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="C38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -4966,13 +4966,13 @@
         <v>99</v>
       </c>
       <c r="B39">
-        <v>2013</v>
+        <v>2019</v>
       </c>
       <c r="C39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -4980,13 +4980,13 @@
         <v>99</v>
       </c>
       <c r="B40">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="C40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -4994,10 +4994,10 @@
         <v>19</v>
       </c>
       <c r="B41">
-        <v>2014</v>
+        <v>2019</v>
       </c>
       <c r="C41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -5008,10 +5008,10 @@
         <v>2019</v>
       </c>
       <c r="C42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -5022,13 +5022,13 @@
         <v>2020</v>
       </c>
       <c r="C43" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
@@ -5036,21 +5036,21 @@
         <v>102</v>
       </c>
       <c r="B44">
-        <v>2000</v>
+        <v>2020</v>
       </c>
       <c r="C44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>103</v>
+        <v>168</v>
       </c>
       <c r="B45">
-        <v>1993</v>
+        <v>2020</v>
       </c>
       <c r="C45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
@@ -5058,29 +5058,29 @@
         <v>12</v>
       </c>
       <c r="B46">
-        <v>2014</v>
+        <v>2020</v>
       </c>
       <c r="C46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B47">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="C47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D47" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:E47">
-    <sortCondition ref="A4:A47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:B47">
+    <sortCondition ref="B3:B47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5097,12 +5097,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
@@ -5112,12 +5112,12 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>